<commit_message>
cleaned airbnb listing file and created new csv
</commit_message>
<xml_diff>
--- a/Resources/Airbnb_Data_Deep_Dive.xlsx
+++ b/Resources/Airbnb_Data_Deep_Dive.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golfz\Documents\GitHub\Eat.Sleep.Data\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\BootCamp\Eat.Sleep.Data\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0D4A64A-39FD-4713-87C9-AC6A8E55BADA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAC5A9B-8347-442B-9BBF-A04BBC71A0DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9A0E361F-336D-4D6B-8DC2-A799C18F4834}"/>
+    <workbookView xWindow="41595" yWindow="-120" windowWidth="15660" windowHeight="13665" xr2:uid="{9A0E361F-336D-4D6B-8DC2-A799C18F4834}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields Required" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
   <si>
     <t>Columns/Fields Required</t>
   </si>
@@ -462,6 +453,15 @@
   </si>
   <si>
     <t>strict_14_with_grace_period</t>
+  </si>
+  <si>
+    <t>We need this - it is the link between the different databases</t>
+  </si>
+  <si>
+    <t>could calculate how many days and see if it is relevant as to how long a host</t>
+  </si>
+  <si>
+    <t>maybe more experienced host with multiple listings does a better or worse job?</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,6 +484,13 @@
       <u/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,6 +535,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -847,7 +858,7 @@
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1391,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1454,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A0B774-F3A5-4AD4-AC99-B7EB72B0FE89}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,8 +1484,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1671,7 +1685,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,8 +1703,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,6 +1718,9 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>